<commit_message>
update to ER data wrangling
</commit_message>
<xml_diff>
--- a/Resources/nst-est2019-01.xlsx
+++ b/Resources/nst-est2019-01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Shared\ESTIMATES\V2019\Team Specific Material\Dissemination\Products\DISS\National-State-Commonwealth Totals\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/topiaslemetyinen/DREAM_Project/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF97A01-FE30-EA49-8EE6-1706E088CF34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="720" yWindow="270" windowWidth="11100" windowHeight="5325"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="16220" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NST01" sheetId="1" r:id="rId1"/>
@@ -62,669 +63,6 @@
     <t>Population Estimate (as of July 1)</t>
   </si>
   <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Alabama</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Alaska</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Arizona</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Arkansas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>California</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Colorado</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Connecticut</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Delaware</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>District of Columbia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Florida</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Georgia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Hawaii</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Idaho</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Illinois</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Indiana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Iowa</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Kansas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Kentucky</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Louisiana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Maine</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Maryland</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Massachusetts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Michigan</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Minnesota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Mississippi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Missouri</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Montana</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Nebraska</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Nevada</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Hampshire</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Jersey</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New Mexico</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>New York</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>North Carolina</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>North Dakota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Ohio</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Oklahoma</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Oregon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Pennsylvania</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Rhode Island</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>South Carolina</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>South Dakota</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Tennessee</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Texas</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Utah</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Vermont</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Virginia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Washington</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>West Virginia</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Wisconsin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="MS sans serif"/>
-      </rPr>
-      <t>Wyoming</t>
-    </r>
-  </si>
-  <si>
     <t>Note: The estimates are based on the 2010 Census and reflect changes to the April 1, 2010 population due to the Count Question Resolution program and geographic program revisions. See Geographic Terms and Definitions at http://www.census.gov/programs-surveys/popest/guidance-geographies/terms-and-definitions.html for a list of the states that are included in each region.  All geographic boundaries for the 2019 population estimates series except statistical area delineations are as of January 1, 2019.  For population estimates methodology statements, see http://www.census.gov/programs-surveys/popest/technical-documentation/methodology.html.</t>
   </si>
   <si>
@@ -738,16 +76,169 @@
   </si>
   <si>
     <t>Release Date: December 2019</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1102,6 +593,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1195,6 +689,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1230,6 +741,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1405,23 +933,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
+      <pane ySplit="4" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
-    <col min="2" max="13" width="14.7109375" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
+    <col min="2" max="13" width="14.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="2.25" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>6</v>
       </c>
@@ -1438,7 +966,7 @@
       <c r="L1" s="22"/>
       <c r="M1" s="22"/>
     </row>
-    <row r="2" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="25.5" customHeight="1">
       <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
@@ -1455,7 +983,7 @@
       <c r="L2" s="24"/>
       <c r="M2" s="24"/>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="2" customFormat="1">
       <c r="A3" s="25" t="s">
         <v>8</v>
       </c>
@@ -1476,7 +1004,7 @@
       <c r="L3" s="28"/>
       <c r="M3" s="28"/>
     </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="3" customFormat="1">
       <c r="A4" s="26"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
@@ -1515,7 +1043,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1084,7 @@
         <v>328239523</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1125,7 @@
         <v>55982803</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1638,7 +1166,7 @@
         <v>68329004</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
@@ -1679,7 +1207,7 @@
         <v>125580448</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="9" t="s">
         <v>4</v>
       </c>
@@ -1720,9 +1248,9 @@
         <v>78347268</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>12</v>
+    <row r="10" spans="1:13">
+      <c r="A10" s="33" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="8">
         <v>4779736</v>
@@ -1761,9 +1289,9 @@
         <v>4903185</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>13</v>
+    <row r="11" spans="1:13">
+      <c r="A11" s="33" t="s">
+        <v>18</v>
       </c>
       <c r="B11" s="8">
         <v>710231</v>
@@ -1802,9 +1330,9 @@
         <v>731545</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>14</v>
+    <row r="12" spans="1:13">
+      <c r="A12" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="B12" s="8">
         <v>6392017</v>
@@ -1843,9 +1371,9 @@
         <v>7278717</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>15</v>
+    <row r="13" spans="1:13">
+      <c r="A13" s="33" t="s">
+        <v>20</v>
       </c>
       <c r="B13" s="8">
         <v>2915918</v>
@@ -1884,9 +1412,9 @@
         <v>3017804</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>16</v>
+    <row r="14" spans="1:13">
+      <c r="A14" s="33" t="s">
+        <v>21</v>
       </c>
       <c r="B14" s="8">
         <v>37253956</v>
@@ -1925,9 +1453,9 @@
         <v>39512223</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>17</v>
+    <row r="15" spans="1:13">
+      <c r="A15" s="33" t="s">
+        <v>22</v>
       </c>
       <c r="B15" s="8">
         <v>5029196</v>
@@ -1966,9 +1494,9 @@
         <v>5758736</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>18</v>
+    <row r="16" spans="1:13">
+      <c r="A16" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="8">
         <v>3574097</v>
@@ -2007,9 +1535,9 @@
         <v>3565287</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>19</v>
+    <row r="17" spans="1:13">
+      <c r="A17" s="33" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="8">
         <v>897934</v>
@@ -2048,9 +1576,9 @@
         <v>973764</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>20</v>
+    <row r="18" spans="1:13">
+      <c r="A18" s="33" t="s">
+        <v>25</v>
       </c>
       <c r="B18" s="8">
         <v>601723</v>
@@ -2089,9 +1617,9 @@
         <v>705749</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>21</v>
+    <row r="19" spans="1:13">
+      <c r="A19" s="33" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="8">
         <v>18801310</v>
@@ -2130,9 +1658,9 @@
         <v>21477737</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>22</v>
+    <row r="20" spans="1:13">
+      <c r="A20" s="33" t="s">
+        <v>27</v>
       </c>
       <c r="B20" s="8">
         <v>9687653</v>
@@ -2171,9 +1699,9 @@
         <v>10617423</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>23</v>
+    <row r="21" spans="1:13">
+      <c r="A21" s="33" t="s">
+        <v>28</v>
       </c>
       <c r="B21" s="8">
         <v>1360301</v>
@@ -2212,9 +1740,9 @@
         <v>1415872</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>24</v>
+    <row r="22" spans="1:13">
+      <c r="A22" s="33" t="s">
+        <v>29</v>
       </c>
       <c r="B22" s="8">
         <v>1567582</v>
@@ -2253,9 +1781,9 @@
         <v>1787065</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>25</v>
+    <row r="23" spans="1:13">
+      <c r="A23" s="33" t="s">
+        <v>30</v>
       </c>
       <c r="B23" s="8">
         <v>12830632</v>
@@ -2294,9 +1822,9 @@
         <v>12671821</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>26</v>
+    <row r="24" spans="1:13">
+      <c r="A24" s="33" t="s">
+        <v>31</v>
       </c>
       <c r="B24" s="8">
         <v>6483802</v>
@@ -2335,9 +1863,9 @@
         <v>6732219</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>27</v>
+    <row r="25" spans="1:13">
+      <c r="A25" s="33" t="s">
+        <v>32</v>
       </c>
       <c r="B25" s="8">
         <v>3046355</v>
@@ -2376,9 +1904,9 @@
         <v>3155070</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>28</v>
+    <row r="26" spans="1:13">
+      <c r="A26" s="33" t="s">
+        <v>33</v>
       </c>
       <c r="B26" s="8">
         <v>2853118</v>
@@ -2417,9 +1945,9 @@
         <v>2913314</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>29</v>
+    <row r="27" spans="1:13">
+      <c r="A27" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="B27" s="8">
         <v>4339367</v>
@@ -2458,9 +1986,9 @@
         <v>4467673</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>30</v>
+    <row r="28" spans="1:13">
+      <c r="A28" s="33" t="s">
+        <v>35</v>
       </c>
       <c r="B28" s="8">
         <v>4533372</v>
@@ -2499,9 +2027,9 @@
         <v>4648794</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>31</v>
+    <row r="29" spans="1:13">
+      <c r="A29" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="B29" s="8">
         <v>1328361</v>
@@ -2540,9 +2068,9 @@
         <v>1344212</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>32</v>
+    <row r="30" spans="1:13">
+      <c r="A30" s="33" t="s">
+        <v>37</v>
       </c>
       <c r="B30" s="8">
         <v>5773552</v>
@@ -2581,9 +2109,9 @@
         <v>6045680</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>33</v>
+    <row r="31" spans="1:13">
+      <c r="A31" s="33" t="s">
+        <v>38</v>
       </c>
       <c r="B31" s="8">
         <v>6547629</v>
@@ -2622,9 +2150,9 @@
         <v>6892503</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>34</v>
+    <row r="32" spans="1:13">
+      <c r="A32" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="B32" s="8">
         <v>9883640</v>
@@ -2663,9 +2191,9 @@
         <v>9986857</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>35</v>
+    <row r="33" spans="1:13">
+      <c r="A33" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="B33" s="8">
         <v>5303925</v>
@@ -2704,9 +2232,9 @@
         <v>5639632</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>36</v>
+    <row r="34" spans="1:13">
+      <c r="A34" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="B34" s="8">
         <v>2967297</v>
@@ -2745,9 +2273,9 @@
         <v>2976149</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>37</v>
+    <row r="35" spans="1:13">
+      <c r="A35" s="33" t="s">
+        <v>42</v>
       </c>
       <c r="B35" s="8">
         <v>5988927</v>
@@ -2786,9 +2314,9 @@
         <v>6137428</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>38</v>
+    <row r="36" spans="1:13">
+      <c r="A36" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="B36" s="8">
         <v>989415</v>
@@ -2827,9 +2355,9 @@
         <v>1068778</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>39</v>
+    <row r="37" spans="1:13">
+      <c r="A37" s="33" t="s">
+        <v>44</v>
       </c>
       <c r="B37" s="8">
         <v>1826341</v>
@@ -2868,9 +2396,9 @@
         <v>1934408</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>40</v>
+    <row r="38" spans="1:13">
+      <c r="A38" s="33" t="s">
+        <v>45</v>
       </c>
       <c r="B38" s="8">
         <v>2700551</v>
@@ -2909,9 +2437,9 @@
         <v>3080156</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>41</v>
+    <row r="39" spans="1:13">
+      <c r="A39" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="B39" s="8">
         <v>1316470</v>
@@ -2950,9 +2478,9 @@
         <v>1359711</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>42</v>
+    <row r="40" spans="1:13">
+      <c r="A40" s="33" t="s">
+        <v>47</v>
       </c>
       <c r="B40" s="8">
         <v>8791894</v>
@@ -2991,9 +2519,9 @@
         <v>8882190</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>43</v>
+    <row r="41" spans="1:13">
+      <c r="A41" s="33" t="s">
+        <v>48</v>
       </c>
       <c r="B41" s="8">
         <v>2059179</v>
@@ -3032,9 +2560,9 @@
         <v>2096829</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
-        <v>44</v>
+    <row r="42" spans="1:13">
+      <c r="A42" s="33" t="s">
+        <v>49</v>
       </c>
       <c r="B42" s="8">
         <v>19378102</v>
@@ -3073,9 +2601,9 @@
         <v>19453561</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>45</v>
+    <row r="43" spans="1:13">
+      <c r="A43" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="B43" s="8">
         <v>9535483</v>
@@ -3114,9 +2642,9 @@
         <v>10488084</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>46</v>
+    <row r="44" spans="1:13">
+      <c r="A44" s="33" t="s">
+        <v>51</v>
       </c>
       <c r="B44" s="8">
         <v>672591</v>
@@ -3155,9 +2683,9 @@
         <v>762062</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>47</v>
+    <row r="45" spans="1:13">
+      <c r="A45" s="33" t="s">
+        <v>52</v>
       </c>
       <c r="B45" s="8">
         <v>11536504</v>
@@ -3196,9 +2724,9 @@
         <v>11689100</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>48</v>
+    <row r="46" spans="1:13">
+      <c r="A46" s="33" t="s">
+        <v>53</v>
       </c>
       <c r="B46" s="8">
         <v>3751351</v>
@@ -3237,9 +2765,9 @@
         <v>3956971</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>49</v>
+    <row r="47" spans="1:13">
+      <c r="A47" s="33" t="s">
+        <v>54</v>
       </c>
       <c r="B47" s="8">
         <v>3831074</v>
@@ -3278,9 +2806,9 @@
         <v>4217737</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>50</v>
+    <row r="48" spans="1:13">
+      <c r="A48" s="33" t="s">
+        <v>55</v>
       </c>
       <c r="B48" s="8">
         <v>12702379</v>
@@ -3319,9 +2847,9 @@
         <v>12801989</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>51</v>
+    <row r="49" spans="1:13">
+      <c r="A49" s="33" t="s">
+        <v>56</v>
       </c>
       <c r="B49" s="8">
         <v>1052567</v>
@@ -3360,9 +2888,9 @@
         <v>1059361</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>52</v>
+    <row r="50" spans="1:13">
+      <c r="A50" s="33" t="s">
+        <v>57</v>
       </c>
       <c r="B50" s="8">
         <v>4625364</v>
@@ -3401,9 +2929,9 @@
         <v>5148714</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>53</v>
+    <row r="51" spans="1:13">
+      <c r="A51" s="33" t="s">
+        <v>58</v>
       </c>
       <c r="B51" s="8">
         <v>814180</v>
@@ -3442,9 +2970,9 @@
         <v>884659</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
-        <v>54</v>
+    <row r="52" spans="1:13">
+      <c r="A52" s="33" t="s">
+        <v>59</v>
       </c>
       <c r="B52" s="8">
         <v>6346105</v>
@@ -3483,9 +3011,9 @@
         <v>6829174</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>55</v>
+    <row r="53" spans="1:13">
+      <c r="A53" s="33" t="s">
+        <v>60</v>
       </c>
       <c r="B53" s="8">
         <v>25145561</v>
@@ -3524,9 +3052,9 @@
         <v>28995881</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>56</v>
+    <row r="54" spans="1:13">
+      <c r="A54" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B54" s="8">
         <v>2763885</v>
@@ -3565,9 +3093,9 @@
         <v>3205958</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
-        <v>57</v>
+    <row r="55" spans="1:13">
+      <c r="A55" s="33" t="s">
+        <v>62</v>
       </c>
       <c r="B55" s="8">
         <v>625741</v>
@@ -3606,9 +3134,9 @@
         <v>623989</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
-        <v>58</v>
+    <row r="56" spans="1:13">
+      <c r="A56" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="B56" s="8">
         <v>8001024</v>
@@ -3647,9 +3175,9 @@
         <v>8535519</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>59</v>
+    <row r="57" spans="1:13">
+      <c r="A57" s="33" t="s">
+        <v>64</v>
       </c>
       <c r="B57" s="8">
         <v>6724540</v>
@@ -3688,9 +3216,9 @@
         <v>7614893</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>60</v>
+    <row r="58" spans="1:13">
+      <c r="A58" s="33" t="s">
+        <v>65</v>
       </c>
       <c r="B58" s="8">
         <v>1852994</v>
@@ -3729,9 +3257,9 @@
         <v>1792147</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>61</v>
+    <row r="59" spans="1:13">
+      <c r="A59" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="B59" s="8">
         <v>5686986</v>
@@ -3770,9 +3298,9 @@
         <v>5822434</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>62</v>
+    <row r="60" spans="1:13">
+      <c r="A60" s="33" t="s">
+        <v>67</v>
       </c>
       <c r="B60" s="8">
         <v>563626</v>
@@ -3811,7 +3339,7 @@
         <v>578759</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" s="11"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -3826,7 +3354,7 @@
       <c r="L61" s="8"/>
       <c r="M61" s="8"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="A62" s="12" t="s">
         <v>5</v>
       </c>
@@ -3867,9 +3395,9 @@
         <v>3193694</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="36" customHeight="1">
       <c r="A63" s="30" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="B63" s="31"/>
       <c r="C63" s="31"/>
@@ -3884,9 +3412,9 @@
       <c r="L63" s="31"/>
       <c r="M63" s="32"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" s="13" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B64" s="14"/>
       <c r="C64" s="14"/>
@@ -3901,9 +3429,9 @@
       <c r="L64" s="14"/>
       <c r="M64" s="15"/>
     </row>
-    <row r="65" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="12.75" customHeight="1">
       <c r="A65" s="16" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -3918,9 +3446,9 @@
       <c r="L65" s="17"/>
       <c r="M65" s="18"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" s="16" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -3935,9 +3463,9 @@
       <c r="L66" s="17"/>
       <c r="M66" s="18"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" s="19" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="B67" s="20"/>
       <c r="C67" s="20"/>

</xml_diff>